<commit_message>
bug fixes all over the place.
</commit_message>
<xml_diff>
--- a/src/main/resources/data/data_30032020/Direct costs2019.xlsx
+++ b/src/main/resources/data/data_30032020/Direct costs2019.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10308"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/datskopetrunov/Downloads/trains/src/main/resources/data/data_30032020/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2EA72F-0765-3D49-8699-DB655A23DA26}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="19200" windowHeight="7875"/>
+    <workbookView xWindow="7360" yWindow="4200" windowWidth="30220" windowHeight="17760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Direct_costs_for_Бруто_тонаже_електрифицираних_теретних_линија</t>
   </si>
@@ -52,12 +58,18 @@
   </si>
   <si>
     <t>Direct_costs_for_Воз_клм_теретних__неелектрификованих_локалних_линија</t>
+  </si>
+  <si>
+    <t>Header row description</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -150,7 +162,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -183,9 +195,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -218,6 +247,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -393,112 +439,120 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="110.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="110.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>6</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>1254838669</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>207115472</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>7</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>1156016670</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>0</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>744191265</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>1060486798</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>2</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>113859100</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>663681979</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
         <v>3</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>716008340</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>10</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>65321839</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
         <v>4</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>14353003</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
-      <c r="B11">
+      <c r="B12">
         <v>18851642</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
         <v>5</v>
       </c>
-      <c r="B12">
+      <c r="B13">
         <v>32421644</v>
       </c>
     </row>
@@ -508,24 +562,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>